<commit_message>
BB0103 AchievementRegistrationReminderMail - A new batch.
</commit_message>
<xml_diff>
--- a/skrum_docs/01_WBS/GoFor0817_20170804.xlsx
+++ b/skrum_docs/01_WBS/GoFor0817_20170804.xlsx
@@ -417,24 +417,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>・ユーザヒアリング
-・資金調達活動
-・コーポレートサイト</t>
-    <rPh sb="11" eb="15">
-      <t>シキn</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>カツド</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・User hearing.
-・Make a document of funding from VC.
-・Make a corporate site.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>・User hearing.
 ・Make a document of funding from VC.
 ・Registration procedure of a company.
@@ -469,19 +451,6 @@
   </si>
   <si>
     <t>・Display selected okr map.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・テストデータ作成
-・進捗登録促進メールバッチ</t>
-    <rPh sb="7" eb="9">
-      <t>サクセ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・Create a complete test data.
-・Achievement encounragement mail batch.</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -697,6 +666,127 @@
 ・Mail sending batch.
 ・Achievement notification mail batch.
 ・Feedback target employees extraction mail batch.</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">・テストデータ作成
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic (本文)"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>・進捗登録促進メールバッチ</t>
+    </r>
+    <rPh sb="7" eb="9">
+      <t>サクセ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>・Create a complete test data.</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic (本文)"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">
+・Achievement encounragement mail batch.</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic (本文)"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>・ユーザヒアリング</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic (本文)"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>・資金調達活動</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+・コーポレートサイト</t>
+    </r>
+    <rPh sb="11" eb="15">
+      <t>シキn</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>カツド</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic (本文)"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>・User hearing.
+・Make a document of funding from VC.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+・Make a corporate site.</t>
     </r>
     <phoneticPr fontId="1"/>
   </si>
@@ -1756,10 +1846,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>14</v>
@@ -1836,10 +1926,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>15</v>
@@ -1862,10 +1952,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>14</v>
@@ -2068,19 +2158,19 @@
         <v>33</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G21" s="9" t="s">
         <v>15</v>
@@ -2100,19 +2190,19 @@
         <v>38</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
ImageUpload - Changed file name from 'image' to '1'
</commit_message>
<xml_diff>
--- a/skrum_docs/01_WBS/GoFor0817_20170804.xlsx
+++ b/skrum_docs/01_WBS/GoFor0817_20170804.xlsx
@@ -795,7 +795,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -848,6 +848,14 @@
       <color rgb="FFFF0000"/>
       <name val="Yu Gothic (本文)"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -921,7 +929,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -982,6 +990,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1006,8 +1015,8 @@
       <xdr:rowOff>79374</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>968375</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1143000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>746125</xdr:rowOff>
     </xdr:to>
@@ -1018,8 +1027,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1952624" y="79374"/>
-          <a:ext cx="10842626" cy="666751"/>
+          <a:off x="1691568" y="79374"/>
+          <a:ext cx="10683876" cy="666751"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1738,14 +1747,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="3" width="24.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="24.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="24.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="12.7109375" style="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="3" width="24.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="1" customWidth="1"/>
+    <col min="5" max="6" width="24.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" style="1" customWidth="1"/>
+    <col min="8" max="9" width="24.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="14.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="64" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1779,7 +1788,7 @@
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -1788,7 +1797,7 @@
       <c r="F3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="22" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -1797,7 +1806,7 @@
       <c r="I3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="22" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1841,7 +1850,7 @@
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="140" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="160" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -2040,10 +2049,10 @@
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="16"/>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="20" t="s">
         <v>37</v>
       </c>
       <c r="G15" s="8" t="s">
@@ -2053,7 +2062,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="120" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="140" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>19</v>
       </c>
@@ -2113,7 +2122,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10" ht="40" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>25</v>
       </c>
@@ -2153,7 +2162,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:10" ht="180" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="220" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
AH0204 AdditionalpathsSearch - Fixed a bug.
</commit_message>
<xml_diff>
--- a/skrum_docs/01_WBS/GoFor0817_20170804.xlsx
+++ b/skrum_docs/01_WBS/GoFor0817_20170804.xlsx
@@ -987,10 +987,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1762,21 +1762,21 @@
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
     </row>
     <row r="3" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -1788,7 +1788,7 @@
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -1797,7 +1797,7 @@
       <c r="F3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="21" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -1806,7 +1806,7 @@
       <c r="I3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="21" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1980,10 +1980,10 @@
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="20" t="s">
         <v>44</v>
       </c>
       <c r="D12" s="8" t="s">

</xml_diff>

<commit_message>
AM0801 CsvUpload - A new api.
</commit_message>
<xml_diff>
--- a/skrum_docs/01_WBS/GoFor0817_20170804.xlsx
+++ b/skrum_docs/01_WBS/GoFor0817_20170804.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="460" windowWidth="27780" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="1060" yWindow="460" windowWidth="27740" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -589,10 +589,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">・EC2とRDSの設定、およびデプロイ
-</t>
-    </r>
-    <r>
       <rPr>
         <strike/>
         <sz val="12"/>
@@ -601,7 +597,7 @@
         <family val="3"/>
         <charset val="128"/>
       </rPr>
-      <t>・目標進捗率集計バッチ</t>
+      <t>・ユーザヒアリング</t>
     </r>
     <r>
       <rPr>
@@ -624,35 +620,29 @@
         <family val="3"/>
         <charset val="128"/>
       </rPr>
-      <t>・メール送信バッチ
-・進捗通知メールバッチ
-・FB対象者抽出メールバッチ</t>
-    </r>
-    <rPh sb="9" eb="11">
-      <t>セッテ</t>
-    </rPh>
-    <rPh sb="21" eb="26">
-      <t>モクヒョ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>シュ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>ソウシn</t>
-    </rPh>
-    <rPh sb="43" eb="45">
-      <t>シンチョk</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>ツウt</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">・Setting EC2 and RDS, and deploy an application.
-</t>
-    </r>
+      <t>・資金調達活動</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+・コーポレートサイト</t>
+    </r>
+    <rPh sb="11" eb="15">
+      <t>シキn</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>カツド</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <r>
       <rPr>
         <strike/>
@@ -662,16 +652,26 @@
         <family val="3"/>
         <charset val="128"/>
       </rPr>
-      <t>・Achievement rate collection batch.
-・Mail sending batch.
-・Achievement notification mail batch.
-・Feedback target employees extraction mail batch.</t>
-    </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">・テストデータ作成
+      <t>・User hearing.
+・Make a document of funding from VC.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+・Make a corporate site.</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">・EC2とRDSの設定、およびデプロイ
 </t>
     </r>
     <r>
@@ -683,42 +683,7 @@
         <family val="3"/>
         <charset val="128"/>
       </rPr>
-      <t>・進捗登録促進メールバッチ</t>
-    </r>
-    <rPh sb="7" eb="9">
-      <t>サクセ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t>・Create a complete test data.</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic (本文)"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">
-・Achievement encounragement mail batch.</t>
-    </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic (本文)"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>・ユーザヒアリング</t>
+      <t>・目標進捗率集計バッチ</t>
     </r>
     <r>
       <rPr>
@@ -741,29 +706,32 @@
         <family val="3"/>
         <charset val="128"/>
       </rPr>
-      <t>・資金調達活動</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-・コーポレートサイト</t>
-    </r>
-    <rPh sb="11" eb="15">
-      <t>シキn</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>カツド</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
+      <t xml:space="preserve">・メール送信バッチ
+・メンバー進捗状況レポートバッチ
+・FB対象者抽出メールバッチ </t>
+    </r>
+    <rPh sb="9" eb="11">
+      <t>セッテ</t>
+    </rPh>
+    <rPh sb="21" eb="26">
+      <t>モクヒョ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>シュ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>ソウシn</t>
+    </rPh>
+    <rPh sb="47" eb="51">
+      <t>シンチョk</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">・Setting EC2 and RDS, and deploy an application.
+</t>
+    </r>
     <r>
       <rPr>
         <strike/>
@@ -773,21 +741,96 @@
         <family val="3"/>
         <charset val="128"/>
       </rPr>
-      <t>・User hearing.
-・Make a document of funding from VC.</t>
+      <t>・Achievement rate collection batch.
+・Email sending batch.
+・Member achievement notification report batch.
+・Feedback target employees extraction email batch.</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>・Create a complete test data.</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic (本文)"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">
+・Achievement encounragement email batch.
+・Member achievement notification report batch.
+・Post notice email.
+・CSV Import api.
+</t>
     </r>
     <r>
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Yu Gothic"/>
-        <family val="2"/>
+        <rFont val="Yu Gothic (本文)"/>
+        <family val="3"/>
         <charset val="128"/>
-        <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">
-・Make a corporate site.</t>
-    </r>
+      <t>・CSV registration batch.</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">・テストデータ作成
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic (本文)"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">・進捗登録促進メールバッチ
+・グループ進捗状況レポートバッチ
+・タイムライン投稿通知メール
+・CSV登録API
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic (本文)"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>・CSV登録バッチ</t>
+    </r>
+    <rPh sb="7" eb="9">
+      <t>サクセ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>シンチョk</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>ジョウky</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>トウコ</t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t>ツウt</t>
+    </rPh>
+    <rPh sb="60" eb="62">
+      <t>トウロk</t>
+    </rPh>
+    <rPh sb="70" eb="72">
+      <t>トウロk</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1739,7 +1782,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight"/>
@@ -1747,14 +1790,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="3" width="24.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="1" customWidth="1"/>
-    <col min="5" max="6" width="24.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5" style="1" customWidth="1"/>
-    <col min="8" max="9" width="24.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="14.83203125" style="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="3" width="24.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="24.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="24.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="12.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="64" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1850,7 +1893,7 @@
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="160" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="140" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -2062,7 +2105,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="140" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="120" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>19</v>
       </c>
@@ -2122,7 +2165,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="40" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>25</v>
       </c>
@@ -2162,24 +2205,24 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:10" ht="220" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="202" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G21" s="9" t="s">
         <v>15</v>
@@ -2199,10 +2242,10 @@
         <v>38</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Map - Added a specific okr's map.
</commit_message>
<xml_diff>
--- a/skrum_docs/01_WBS/GoFor0817_20170804.xlsx
+++ b/skrum_docs/01_WBS/GoFor0817_20170804.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="460" windowWidth="27580" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="1280" yWindow="460" windowWidth="27520" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -813,7 +813,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -864,6 +864,15 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Yu Gothic"/>
       <family val="2"/>
       <charset val="128"/>
@@ -941,7 +950,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -999,6 +1008,9 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1634,10 +1646,10 @@
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="17" t="s">
         <v>43</v>
       </c>
       <c r="G7" s="8" t="s">
@@ -1668,10 +1680,10 @@
       <c r="B9" s="13"/>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="17" t="s">
         <v>43</v>
       </c>
       <c r="G9" s="8" t="s">
@@ -1685,10 +1697,10 @@
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="22" t="s">
         <v>57</v>
       </c>
       <c r="D10" s="9" t="s">

</xml_diff>